<commit_message>
Array Problems Day 2 commit
</commit_message>
<xml_diff>
--- a/AlgosDS/src/com/leetcode/leetcode-tracker.xlsx
+++ b/AlgosDS/src/com/leetcode/leetcode-tracker.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Two Sum</t>
   </si>
@@ -437,7 +437,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,6 +479,9 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -548,6 +551,9 @@
       <c r="C9" t="s">
         <v>15</v>
       </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -569,6 +575,9 @@
       </c>
       <c r="C11" t="s">
         <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
String challenge commit 1
</commit_message>
<xml_diff>
--- a/AlgosDS/src/com/leetcode/leetcode-tracker.xlsx
+++ b/AlgosDS/src/com/leetcode/leetcode-tracker.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="String" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Two Sum</t>
   </si>
@@ -96,6 +96,66 @@
   </si>
   <si>
     <t xml:space="preserve"> -  https://www.geeksforgeeks.org/binary-search/</t>
+  </si>
+  <si>
+    <t>Longest Substring Without Repeating Characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - https://leetcode.com/problems/longest-substring-without-repeating-characters/</t>
+  </si>
+  <si>
+    <t>Longest Repeating Character Replacement</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - https://leetcode.com/problems/longest-repeating-character-replacement/</t>
+  </si>
+  <si>
+    <t>Minimum Window Substring</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - https://leetcode.com/problems/minimum-window-substring/</t>
+  </si>
+  <si>
+    <t>Valid Anagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - https://leetcode.com/problems/valid-anagram/</t>
+  </si>
+  <si>
+    <t>Group Anagrams</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - https://leetcode.com/problems/group-anagrams/</t>
+  </si>
+  <si>
+    <t>Valid Parentheses</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - https://leetcode.com/problems/valid-parentheses/</t>
+  </si>
+  <si>
+    <t>Valid Palindrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - https://leetcode.com/problems/valid-palindrome/</t>
+  </si>
+  <si>
+    <t>Longest Palindromic Substring</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - https://leetcode.com/problems/longest-palindromic-substring/</t>
+  </si>
+  <si>
+    <t>Palindromic Substrings</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - https://leetcode.com/problems/palindromic-substrings/</t>
+  </si>
+  <si>
+    <t>Encode and Decode Strings (Leetcode Premium)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - https://leetcode.com/problems/encode-and-decode-strings/</t>
   </si>
 </sst>
 </file>
@@ -436,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,12 +681,108 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>